<commit_message>
inventory update; TLC pin defs changed
I changed what port on the TLC59711 goes to which board to make routing
the Micro RevB easier. Tried to make an Accel, but there appears to be
shorts....
</commit_message>
<xml_diff>
--- a/Inventory and Acquisitions/Master Inventory.xlsx
+++ b/Inventory and Acquisitions/Master Inventory.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="160">
   <si>
     <t>Inventory for TESA Project</t>
   </si>
@@ -897,8 +897,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1307,7 +1307,7 @@
         <v>10</v>
       </c>
       <c r="B18">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C18" t="s">
         <v>65</v>
@@ -1851,8 +1851,8 @@
       <c r="A34" t="s">
         <v>10</v>
       </c>
-      <c r="B34" t="s">
-        <v>157</v>
+      <c r="B34">
+        <v>11</v>
       </c>
       <c r="C34" t="s">
         <v>143</v>

</xml_diff>

<commit_message>
A good day of work!
Assembled a RevB micro, have not yet tested; started making a list of
what I did wrong in this one (stupid me, I forgot the logo, pin 1
designations); readme contains info about jumper resistors used on the
board
</commit_message>
<xml_diff>
--- a/Inventory and Acquisitions/Master Inventory.xlsx
+++ b/Inventory and Acquisitions/Master Inventory.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="212">
   <si>
     <t>Inventory for TESA Project</t>
   </si>
@@ -166,9 +166,6 @@
   </si>
   <si>
     <t>R103</t>
-  </si>
-  <si>
-    <t>R104,R105</t>
   </si>
   <si>
     <t>667-ERJ-3GEYJ220V</t>
@@ -370,9 +367,6 @@
     <t>Board</t>
   </si>
   <si>
-    <t>micro</t>
-  </si>
-  <si>
     <t>micro (1)</t>
   </si>
   <si>
@@ -490,13 +484,175 @@
     <t>C104</t>
   </si>
   <si>
-    <t>Last updated: Oct. 18/14</t>
-  </si>
-  <si>
     <t>C106,C203,C402</t>
   </si>
   <si>
     <t>C101,C102,C103,C107,C201,C202,C301,C401</t>
+  </si>
+  <si>
+    <t>0.253/0.232/--</t>
+  </si>
+  <si>
+    <t>150060VS75000</t>
+  </si>
+  <si>
+    <t>Wurth</t>
+  </si>
+  <si>
+    <t>710-150060VS75000</t>
+  </si>
+  <si>
+    <t>LED4</t>
+  </si>
+  <si>
+    <t>Green LED</t>
+  </si>
+  <si>
+    <t>150060RS75000</t>
+  </si>
+  <si>
+    <t>710-150060RS75000</t>
+  </si>
+  <si>
+    <t>LED5</t>
+  </si>
+  <si>
+    <t>Red LED</t>
+  </si>
+  <si>
+    <t>--/0.437/0.412</t>
+  </si>
+  <si>
+    <t>961110-6404-AR</t>
+  </si>
+  <si>
+    <t>3M</t>
+  </si>
+  <si>
+    <t>517-9611106404AR</t>
+  </si>
+  <si>
+    <t>Pin Headers</t>
+  </si>
+  <si>
+    <t>0.578/0.43/0.317</t>
+  </si>
+  <si>
+    <t>LP2985-33DBVR</t>
+  </si>
+  <si>
+    <t>595-LP2985-33DBVR</t>
+  </si>
+  <si>
+    <t>SOT-23-5</t>
+  </si>
+  <si>
+    <t>U103</t>
+  </si>
+  <si>
+    <t>0.012/0.01/--</t>
+  </si>
+  <si>
+    <t>CRCW06030000Z0EA</t>
+  </si>
+  <si>
+    <t>Vishay</t>
+  </si>
+  <si>
+    <t>71-CRCW0603-0-E3</t>
+  </si>
+  <si>
+    <t>R105,R108</t>
+  </si>
+  <si>
+    <t>0.06/0.036/0.03</t>
+  </si>
+  <si>
+    <t>VJ0603Y103KXAAC</t>
+  </si>
+  <si>
+    <t>77-VJ0603Y103KXAAC</t>
+  </si>
+  <si>
+    <t>C105</t>
+  </si>
+  <si>
+    <t>10n</t>
+  </si>
+  <si>
+    <t>CRCW0603180RJNEA</t>
+  </si>
+  <si>
+    <t>71-CRCW0603J-180-E3</t>
+  </si>
+  <si>
+    <t>R106,R107</t>
+  </si>
+  <si>
+    <t>0.016/0.012/--</t>
+  </si>
+  <si>
+    <t>CRCW06032K00FKEA</t>
+  </si>
+  <si>
+    <t>71-CRCW0603-2.0K-E3</t>
+  </si>
+  <si>
+    <t>R104</t>
+  </si>
+  <si>
+    <t>0.434/0.35/--</t>
+  </si>
+  <si>
+    <t>CSTCE16M0V53-R0</t>
+  </si>
+  <si>
+    <t>81-CSTCE16M0V53-R0</t>
+  </si>
+  <si>
+    <t>16M</t>
+  </si>
+  <si>
+    <t>3.64/2.74/2.58</t>
+  </si>
+  <si>
+    <t>ATMEGA328P-AU</t>
+  </si>
+  <si>
+    <t>556-ATMEGA328P-AU</t>
+  </si>
+  <si>
+    <t>TQFP_32</t>
+  </si>
+  <si>
+    <t>Microcontroller</t>
+  </si>
+  <si>
+    <t>0.063/0.035/--</t>
+  </si>
+  <si>
+    <t>GRM188R60J475KE19D</t>
+  </si>
+  <si>
+    <t>C203</t>
+  </si>
+  <si>
+    <t>4.7u</t>
+  </si>
+  <si>
+    <t>Last updated: Nov. 4/14</t>
+  </si>
+  <si>
+    <t>micro-A</t>
+  </si>
+  <si>
+    <t>micro-B</t>
+  </si>
+  <si>
+    <t>NO (prev R105,R106)</t>
+  </si>
+  <si>
+    <t>2k (mistake)</t>
   </si>
 </sst>
 </file>
@@ -895,10 +1051,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L34"/>
+  <dimension ref="A1:L46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -925,7 +1081,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>157</v>
+        <v>207</v>
       </c>
       <c r="B2" s="2"/>
     </row>
@@ -949,7 +1105,7 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -987,7 +1143,7 @@
         <v>9</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -995,13 +1151,13 @@
         <v>10</v>
       </c>
       <c r="B9">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C9" t="s">
         <v>22</v>
       </c>
       <c r="D9" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E9" t="s">
         <v>12</v>
@@ -1019,13 +1175,13 @@
         <v>16</v>
       </c>
       <c r="J9" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="K9" t="s">
         <v>18</v>
       </c>
       <c r="L9" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -1033,7 +1189,7 @@
         <v>20</v>
       </c>
       <c r="B10">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C10" t="s">
         <v>21</v>
@@ -1057,13 +1213,13 @@
         <v>25</v>
       </c>
       <c r="J10" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="K10" t="s">
         <v>18</v>
       </c>
       <c r="L10" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -1106,7 +1262,7 @@
         <v>36</v>
       </c>
       <c r="B12">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C12" t="s">
         <v>37</v>
@@ -1130,13 +1286,13 @@
         <v>41</v>
       </c>
       <c r="J12" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="K12" t="s">
         <v>18</v>
       </c>
       <c r="L12" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -1168,13 +1324,13 @@
         <v>45</v>
       </c>
       <c r="J13" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="K13" t="s">
         <v>18</v>
       </c>
       <c r="L13" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -1206,13 +1362,13 @@
         <v>48</v>
       </c>
       <c r="J14" s="7" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="K14" s="7" t="s">
         <v>18</v>
       </c>
       <c r="L14" s="7" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -1226,7 +1382,7 @@
         <v>22</v>
       </c>
       <c r="D15" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="E15" t="s">
         <v>12</v>
@@ -1235,22 +1391,22 @@
         <v>13</v>
       </c>
       <c r="G15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H15" t="s">
         <v>24</v>
       </c>
       <c r="I15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J15" t="s">
         <v>26</v>
       </c>
       <c r="K15" s="7" t="s">
-        <v>18</v>
+        <v>210</v>
       </c>
       <c r="L15" s="7" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -1261,7 +1417,7 @@
         <v>10</v>
       </c>
       <c r="C16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D16" t="s">
         <v>49</v>
@@ -1273,22 +1429,22 @@
         <v>13</v>
       </c>
       <c r="G16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H16" t="s">
         <v>24</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J16" s="7" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="K16" s="7" t="s">
         <v>18</v>
       </c>
       <c r="L16" s="7" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -1299,7 +1455,7 @@
         <v>10</v>
       </c>
       <c r="C17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D17" t="s">
         <v>49</v>
@@ -1311,22 +1467,22 @@
         <v>13</v>
       </c>
       <c r="G17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H17" t="s">
         <v>24</v>
       </c>
       <c r="I17" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J17" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="K17" s="7" t="s">
         <v>18</v>
       </c>
       <c r="L17" s="7" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -1334,13 +1490,13 @@
         <v>10</v>
       </c>
       <c r="B18">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D18" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="E18" t="s">
         <v>12</v>
@@ -1349,22 +1505,22 @@
         <v>13</v>
       </c>
       <c r="G18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H18" t="s">
         <v>15</v>
       </c>
       <c r="I18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J18" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="K18" s="7" t="s">
         <v>18</v>
       </c>
       <c r="L18" s="7" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
@@ -1375,130 +1531,130 @@
         <v>12</v>
       </c>
       <c r="C19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D19" t="s">
+        <v>62</v>
+      </c>
+      <c r="E19" t="s">
         <v>63</v>
       </c>
-      <c r="E19" t="s">
-        <v>64</v>
-      </c>
       <c r="F19" s="9" t="s">
         <v>13</v>
       </c>
       <c r="G19" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H19" t="s">
         <v>15</v>
       </c>
       <c r="I19" t="s">
+        <v>105</v>
+      </c>
+      <c r="J19" t="s">
         <v>106</v>
       </c>
-      <c r="J19" t="s">
-        <v>107</v>
-      </c>
       <c r="K19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B20">
         <v>5</v>
       </c>
       <c r="C20" t="s">
+        <v>67</v>
+      </c>
+      <c r="D20" t="s">
         <v>68</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
+        <v>81</v>
+      </c>
+      <c r="F20" t="s">
+        <v>13</v>
+      </c>
+      <c r="G20" t="s">
         <v>69</v>
       </c>
-      <c r="E20" t="s">
-        <v>82</v>
-      </c>
-      <c r="F20" t="s">
-        <v>13</v>
-      </c>
-      <c r="G20" t="s">
+      <c r="H20" t="s">
         <v>70</v>
       </c>
-      <c r="H20" t="s">
+      <c r="I20" t="s">
         <v>71</v>
       </c>
-      <c r="I20" t="s">
-        <v>72</v>
-      </c>
       <c r="J20" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="K20" t="s">
         <v>18</v>
       </c>
       <c r="L20" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B21">
         <v>71</v>
       </c>
       <c r="C21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D21" t="s">
+        <v>73</v>
+      </c>
+      <c r="E21" t="s">
         <v>74</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
+        <v>13</v>
+      </c>
+      <c r="G21" t="s">
         <v>75</v>
       </c>
-      <c r="F21" t="s">
-        <v>13</v>
-      </c>
-      <c r="G21" t="s">
+      <c r="H21" t="s">
         <v>76</v>
       </c>
-      <c r="H21" t="s">
+      <c r="I21" t="s">
         <v>77</v>
       </c>
-      <c r="I21" t="s">
-        <v>78</v>
-      </c>
       <c r="J21" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="K21" t="s">
         <v>18</v>
       </c>
       <c r="L21" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B22">
         <v>7</v>
       </c>
       <c r="C22" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D22" t="s">
+        <v>79</v>
+      </c>
+      <c r="E22" t="s">
         <v>80</v>
       </c>
-      <c r="E22" t="s">
-        <v>81</v>
-      </c>
       <c r="H22" t="s">
+        <v>82</v>
+      </c>
+      <c r="I22" t="s">
         <v>83</v>
-      </c>
-      <c r="I22" t="s">
-        <v>84</v>
       </c>
       <c r="K22" t="s">
         <v>18</v>
@@ -1506,224 +1662,224 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B23">
         <v>4</v>
       </c>
       <c r="C23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D23" t="s">
+        <v>84</v>
+      </c>
+      <c r="E23" t="s">
         <v>85</v>
       </c>
-      <c r="E23" t="s">
+      <c r="F23" t="s">
+        <v>13</v>
+      </c>
+      <c r="G23" t="s">
         <v>86</v>
       </c>
-      <c r="F23" t="s">
-        <v>13</v>
-      </c>
-      <c r="G23" t="s">
+      <c r="H23" t="s">
+        <v>82</v>
+      </c>
+      <c r="I23" t="s">
         <v>87</v>
       </c>
-      <c r="H23" t="s">
-        <v>83</v>
-      </c>
-      <c r="I23" t="s">
-        <v>88</v>
-      </c>
       <c r="J23" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="K23" t="s">
         <v>18</v>
       </c>
       <c r="L23" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B24">
         <v>4</v>
       </c>
       <c r="C24" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D24" t="s">
+        <v>90</v>
+      </c>
+      <c r="E24" t="s">
+        <v>94</v>
+      </c>
+      <c r="F24" t="s">
+        <v>13</v>
+      </c>
+      <c r="G24" t="s">
         <v>91</v>
       </c>
-      <c r="E24" t="s">
-        <v>95</v>
-      </c>
-      <c r="F24" t="s">
-        <v>13</v>
-      </c>
-      <c r="G24" t="s">
+      <c r="H24" t="s">
         <v>92</v>
       </c>
-      <c r="H24" t="s">
+      <c r="I24" t="s">
         <v>93</v>
       </c>
-      <c r="I24" t="s">
-        <v>94</v>
-      </c>
       <c r="J24" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="K24" t="s">
         <v>18</v>
       </c>
       <c r="L24" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B25">
         <v>6</v>
       </c>
       <c r="C25" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D25" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E25" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F25" t="s">
         <v>13</v>
       </c>
       <c r="G25" t="s">
+        <v>96</v>
+      </c>
+      <c r="H25" t="s">
         <v>97</v>
       </c>
-      <c r="H25" t="s">
+      <c r="I25" t="s">
         <v>98</v>
       </c>
-      <c r="I25" t="s">
+      <c r="J25" t="s">
         <v>99</v>
       </c>
-      <c r="J25" t="s">
-        <v>100</v>
-      </c>
       <c r="K25" t="s">
         <v>18</v>
       </c>
       <c r="L25" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B26" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C26" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D26" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E26" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F26" t="s">
         <v>13</v>
       </c>
       <c r="G26" t="s">
+        <v>100</v>
+      </c>
+      <c r="H26" t="s">
         <v>101</v>
       </c>
-      <c r="H26" t="s">
+      <c r="I26" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="I26" s="5" t="s">
+      <c r="J26" t="s">
         <v>103</v>
       </c>
-      <c r="J26" t="s">
-        <v>104</v>
-      </c>
       <c r="K26" t="s">
         <v>18</v>
       </c>
       <c r="L26" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B27" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C27" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D27" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E27" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F27" t="s">
+        <v>110</v>
+      </c>
+      <c r="G27" t="s">
         <v>111</v>
       </c>
-      <c r="G27" t="s">
+      <c r="H27" t="s">
         <v>112</v>
       </c>
-      <c r="H27" t="s">
+      <c r="I27" t="s">
         <v>113</v>
       </c>
-      <c r="I27" t="s">
+      <c r="J27" t="s">
         <v>114</v>
       </c>
-      <c r="J27" t="s">
-        <v>115</v>
-      </c>
       <c r="K27" t="s">
         <v>18</v>
       </c>
       <c r="L27" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B28">
         <v>10</v>
       </c>
       <c r="C28" t="s">
+        <v>208</v>
+      </c>
+      <c r="D28" t="s">
+        <v>116</v>
+      </c>
+      <c r="E28" t="s">
+        <v>62</v>
+      </c>
+      <c r="F28" t="s">
         <v>117</v>
       </c>
-      <c r="D28" t="s">
-        <v>118</v>
-      </c>
-      <c r="E28" t="s">
-        <v>63</v>
-      </c>
-      <c r="F28" t="s">
-        <v>119</v>
-      </c>
       <c r="G28" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H28" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I28" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J28" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K28" t="s">
         <v>18</v>
@@ -1731,34 +1887,34 @@
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B29">
         <v>10</v>
       </c>
       <c r="C29" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D29" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E29" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F29" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="G29" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H29" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I29" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J29" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K29" t="s">
         <v>18</v>
@@ -1766,34 +1922,34 @@
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B30">
         <v>12</v>
       </c>
       <c r="C30" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D30" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E30" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F30" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="G30" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H30" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I30" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J30" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K30" t="s">
         <v>18</v>
@@ -1801,34 +1957,34 @@
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B31">
         <v>11</v>
       </c>
       <c r="C31" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D31" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E31" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F31" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="G31" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H31" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I31" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J31" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K31" t="s">
         <v>18</v>
@@ -1842,10 +1998,10 @@
         <v>11</v>
       </c>
       <c r="C32" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D32" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="E32" t="s">
         <v>12</v>
@@ -1854,60 +2010,60 @@
         <v>13</v>
       </c>
       <c r="G32" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="H32" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="I32" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="J32" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="K32" t="s">
         <v>18</v>
       </c>
       <c r="L32" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B33">
         <v>5</v>
       </c>
       <c r="C33" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D33" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E33" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F33" t="s">
         <v>13</v>
       </c>
       <c r="G33" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="H33" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="I33" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="J33" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="K33" t="s">
         <v>18</v>
       </c>
       <c r="L33" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
@@ -1918,10 +2074,10 @@
         <v>11</v>
       </c>
       <c r="C34" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D34" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="E34" t="s">
         <v>12</v>
@@ -1930,22 +2086,475 @@
         <v>13</v>
       </c>
       <c r="G34" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="H34" t="s">
         <v>15</v>
       </c>
       <c r="I34" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="J34" t="s">
+        <v>142</v>
+      </c>
+      <c r="K34" t="s">
+        <v>18</v>
+      </c>
+      <c r="L34" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>10</v>
+      </c>
+      <c r="B35">
+        <v>10</v>
+      </c>
+      <c r="C35" t="s">
+        <v>206</v>
+      </c>
+      <c r="D35" t="s">
+        <v>205</v>
+      </c>
+      <c r="E35" t="s">
+        <v>12</v>
+      </c>
+      <c r="F35" t="s">
+        <v>13</v>
+      </c>
+      <c r="G35" t="s">
+        <v>126</v>
+      </c>
+      <c r="H35" t="s">
+        <v>15</v>
+      </c>
+      <c r="I35" t="s">
+        <v>204</v>
+      </c>
+      <c r="J35" t="s">
+        <v>203</v>
+      </c>
+      <c r="K35" t="s">
+        <v>18</v>
+      </c>
+      <c r="L35" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>202</v>
+      </c>
+      <c r="B36">
+        <v>5</v>
+      </c>
+      <c r="C36" t="s">
+        <v>62</v>
+      </c>
+      <c r="D36" t="s">
+        <v>79</v>
+      </c>
+      <c r="E36" t="s">
+        <v>201</v>
+      </c>
+      <c r="F36" t="s">
+        <v>13</v>
+      </c>
+      <c r="G36" t="s">
+        <v>200</v>
+      </c>
+      <c r="H36" t="s">
+        <v>82</v>
+      </c>
+      <c r="I36" t="s">
+        <v>199</v>
+      </c>
+      <c r="J36" t="s">
+        <v>198</v>
+      </c>
+      <c r="K36" t="s">
+        <v>18</v>
+      </c>
+      <c r="L36" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>36</v>
+      </c>
+      <c r="B37">
+        <v>4</v>
+      </c>
+      <c r="C37" t="s">
+        <v>197</v>
+      </c>
+      <c r="D37" t="s">
+        <v>38</v>
+      </c>
+      <c r="E37" t="s">
+        <v>39</v>
+      </c>
+      <c r="F37" t="s">
+        <v>13</v>
+      </c>
+      <c r="G37" t="s">
+        <v>196</v>
+      </c>
+      <c r="H37" t="s">
+        <v>15</v>
+      </c>
+      <c r="I37" t="s">
+        <v>195</v>
+      </c>
+      <c r="J37" t="s">
+        <v>194</v>
+      </c>
+      <c r="K37" t="s">
+        <v>18</v>
+      </c>
+      <c r="L37" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>20</v>
+      </c>
+      <c r="B38">
+        <v>9</v>
+      </c>
+      <c r="C38" t="s">
+        <v>211</v>
+      </c>
+      <c r="D38" t="s">
+        <v>193</v>
+      </c>
+      <c r="E38" t="s">
+        <v>12</v>
+      </c>
+      <c r="F38" t="s">
+        <v>13</v>
+      </c>
+      <c r="G38" t="s">
+        <v>192</v>
+      </c>
+      <c r="H38" t="s">
+        <v>179</v>
+      </c>
+      <c r="I38" t="s">
+        <v>191</v>
+      </c>
+      <c r="J38" t="s">
+        <v>190</v>
+      </c>
+      <c r="K38" t="s">
+        <v>18</v>
+      </c>
+      <c r="L38" t="s">
         <v>144</v>
       </c>
-      <c r="K34" t="s">
-        <v>18</v>
-      </c>
-      <c r="L34" t="s">
-        <v>140</v>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>20</v>
+      </c>
+      <c r="B39">
+        <v>12</v>
+      </c>
+      <c r="C39">
+        <v>180</v>
+      </c>
+      <c r="D39" t="s">
+        <v>189</v>
+      </c>
+      <c r="E39" t="s">
+        <v>12</v>
+      </c>
+      <c r="F39" t="s">
+        <v>13</v>
+      </c>
+      <c r="G39" t="s">
+        <v>188</v>
+      </c>
+      <c r="H39" t="s">
+        <v>179</v>
+      </c>
+      <c r="I39" t="s">
+        <v>187</v>
+      </c>
+      <c r="J39" t="s">
+        <v>177</v>
+      </c>
+      <c r="K39" t="s">
+        <v>18</v>
+      </c>
+      <c r="L39" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>10</v>
+      </c>
+      <c r="B40">
+        <v>9</v>
+      </c>
+      <c r="C40" t="s">
+        <v>186</v>
+      </c>
+      <c r="D40" t="s">
+        <v>185</v>
+      </c>
+      <c r="E40" t="s">
+        <v>12</v>
+      </c>
+      <c r="F40" t="s">
+        <v>13</v>
+      </c>
+      <c r="G40" t="s">
+        <v>184</v>
+      </c>
+      <c r="H40" t="s">
+        <v>179</v>
+      </c>
+      <c r="I40" t="s">
+        <v>183</v>
+      </c>
+      <c r="J40" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="K40" t="s">
+        <v>18</v>
+      </c>
+      <c r="L40" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>20</v>
+      </c>
+      <c r="B41">
+        <v>13</v>
+      </c>
+      <c r="C41">
+        <v>0</v>
+      </c>
+      <c r="D41" t="s">
+        <v>181</v>
+      </c>
+      <c r="E41" t="s">
+        <v>12</v>
+      </c>
+      <c r="F41" t="s">
+        <v>13</v>
+      </c>
+      <c r="G41" t="s">
+        <v>180</v>
+      </c>
+      <c r="H41" t="s">
+        <v>179</v>
+      </c>
+      <c r="I41" t="s">
+        <v>178</v>
+      </c>
+      <c r="J41" t="s">
+        <v>177</v>
+      </c>
+      <c r="K41" t="s">
+        <v>18</v>
+      </c>
+      <c r="L41" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>65</v>
+      </c>
+      <c r="B42">
+        <v>4</v>
+      </c>
+      <c r="C42" t="s">
+        <v>67</v>
+      </c>
+      <c r="D42" t="s">
+        <v>176</v>
+      </c>
+      <c r="E42" t="s">
+        <v>175</v>
+      </c>
+      <c r="F42" t="s">
+        <v>13</v>
+      </c>
+      <c r="G42" t="s">
+        <v>174</v>
+      </c>
+      <c r="H42" t="s">
+        <v>128</v>
+      </c>
+      <c r="I42" t="s">
+        <v>173</v>
+      </c>
+      <c r="J42" t="s">
+        <v>172</v>
+      </c>
+      <c r="K42" t="s">
+        <v>18</v>
+      </c>
+      <c r="L42" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>171</v>
+      </c>
+      <c r="B43">
+        <v>5</v>
+      </c>
+      <c r="C43" t="s">
+        <v>62</v>
+      </c>
+      <c r="D43" t="s">
+        <v>62</v>
+      </c>
+      <c r="E43" t="s">
+        <v>62</v>
+      </c>
+      <c r="F43" t="s">
+        <v>13</v>
+      </c>
+      <c r="G43" t="s">
+        <v>170</v>
+      </c>
+      <c r="H43" t="s">
+        <v>169</v>
+      </c>
+      <c r="I43" t="s">
+        <v>168</v>
+      </c>
+      <c r="J43" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="K43" t="s">
+        <v>18</v>
+      </c>
+      <c r="L43" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>166</v>
+      </c>
+      <c r="B44">
+        <v>9</v>
+      </c>
+      <c r="C44" t="s">
+        <v>62</v>
+      </c>
+      <c r="D44" t="s">
+        <v>165</v>
+      </c>
+      <c r="E44" t="s">
+        <v>12</v>
+      </c>
+      <c r="F44" t="s">
+        <v>13</v>
+      </c>
+      <c r="G44" t="s">
+        <v>164</v>
+      </c>
+      <c r="H44" t="s">
+        <v>159</v>
+      </c>
+      <c r="I44" t="s">
+        <v>163</v>
+      </c>
+      <c r="J44" t="s">
+        <v>157</v>
+      </c>
+      <c r="K44" t="s">
+        <v>18</v>
+      </c>
+      <c r="L44" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>162</v>
+      </c>
+      <c r="B45">
+        <v>9</v>
+      </c>
+      <c r="C45" t="s">
+        <v>62</v>
+      </c>
+      <c r="D45" t="s">
+        <v>161</v>
+      </c>
+      <c r="E45" t="s">
+        <v>12</v>
+      </c>
+      <c r="F45" t="s">
+        <v>13</v>
+      </c>
+      <c r="G45" t="s">
+        <v>160</v>
+      </c>
+      <c r="H45" t="s">
+        <v>159</v>
+      </c>
+      <c r="I45" t="s">
+        <v>158</v>
+      </c>
+      <c r="J45" t="s">
+        <v>157</v>
+      </c>
+      <c r="K45" t="s">
+        <v>18</v>
+      </c>
+      <c r="L45" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>115</v>
+      </c>
+      <c r="B46">
+        <v>19</v>
+      </c>
+      <c r="C46" t="s">
+        <v>209</v>
+      </c>
+      <c r="D46" t="s">
+        <v>116</v>
+      </c>
+      <c r="E46" t="s">
+        <v>62</v>
+      </c>
+      <c r="F46" t="s">
+        <v>117</v>
+      </c>
+      <c r="G46" t="s">
+        <v>62</v>
+      </c>
+      <c r="H46" t="s">
+        <v>62</v>
+      </c>
+      <c r="I46" t="s">
+        <v>62</v>
+      </c>
+      <c r="J46" t="s">
+        <v>62</v>
+      </c>
+      <c r="K46" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Partial build of a board
Updated inventory to reflect components used: a very good habit that I'm
trying to develop.
</commit_message>
<xml_diff>
--- a/Inventory and Acquisitions/Master Inventory.xlsx
+++ b/Inventory and Acquisitions/Master Inventory.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="211">
   <si>
     <t>Inventory for TESA Project</t>
   </si>
@@ -575,9 +575,6 @@
   </si>
   <si>
     <t>C105</t>
-  </si>
-  <si>
-    <t>10n</t>
   </si>
   <si>
     <t>CRCW0603180RJNEA</t>
@@ -1053,8 +1050,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1081,7 +1078,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B2" s="2"/>
     </row>
@@ -1262,7 +1259,7 @@
         <v>36</v>
       </c>
       <c r="B12">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C12" t="s">
         <v>37</v>
@@ -1403,7 +1400,7 @@
         <v>26</v>
       </c>
       <c r="K15" s="7" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="L15" s="7" t="s">
         <v>144</v>
@@ -1601,7 +1598,7 @@
         <v>72</v>
       </c>
       <c r="B21">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C21" t="s">
         <v>62</v>
@@ -1858,7 +1855,7 @@
         <v>10</v>
       </c>
       <c r="C28" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D28" t="s">
         <v>116</v>
@@ -2112,10 +2109,10 @@
         <v>10</v>
       </c>
       <c r="C35" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D35" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E35" t="s">
         <v>12</v>
@@ -2130,10 +2127,10 @@
         <v>15</v>
       </c>
       <c r="I35" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="J35" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="K35" t="s">
         <v>18</v>
@@ -2144,10 +2141,10 @@
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B36">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C36" t="s">
         <v>62</v>
@@ -2156,22 +2153,22 @@
         <v>79</v>
       </c>
       <c r="E36" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F36" t="s">
         <v>13</v>
       </c>
       <c r="G36" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H36" t="s">
         <v>82</v>
       </c>
       <c r="I36" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="J36" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K36" t="s">
         <v>18</v>
@@ -2188,7 +2185,7 @@
         <v>4</v>
       </c>
       <c r="C37" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D37" t="s">
         <v>38</v>
@@ -2200,16 +2197,16 @@
         <v>13</v>
       </c>
       <c r="G37" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H37" t="s">
         <v>15</v>
       </c>
       <c r="I37" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J37" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="K37" t="s">
         <v>18</v>
@@ -2226,10 +2223,10 @@
         <v>9</v>
       </c>
       <c r="C38" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D38" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E38" t="s">
         <v>12</v>
@@ -2238,16 +2235,16 @@
         <v>13</v>
       </c>
       <c r="G38" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H38" t="s">
         <v>179</v>
       </c>
       <c r="I38" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="J38" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="K38" t="s">
         <v>18</v>
@@ -2267,7 +2264,7 @@
         <v>180</v>
       </c>
       <c r="D39" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E39" t="s">
         <v>12</v>
@@ -2276,13 +2273,13 @@
         <v>13</v>
       </c>
       <c r="G39" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H39" t="s">
         <v>179</v>
       </c>
       <c r="I39" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="J39" t="s">
         <v>177</v>
@@ -2299,10 +2296,10 @@
         <v>10</v>
       </c>
       <c r="B40">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C40" t="s">
-        <v>186</v>
+        <v>61</v>
       </c>
       <c r="D40" t="s">
         <v>185</v>
@@ -2375,7 +2372,7 @@
         <v>65</v>
       </c>
       <c r="B42">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C42" t="s">
         <v>67</v>
@@ -2530,7 +2527,7 @@
         <v>19</v>
       </c>
       <c r="C46" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D46" t="s">
         <v>116</v>

</xml_diff>

<commit_message>
Update to inventory; added a FW design doc
Also, removed some crappy experimentations I had done for FW.
</commit_message>
<xml_diff>
--- a/Inventory and Acquisitions/Master Inventory.xlsx
+++ b/Inventory and Acquisitions/Master Inventory.xlsx
@@ -1050,8 +1050,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1148,7 +1148,7 @@
         <v>10</v>
       </c>
       <c r="B9">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C9" t="s">
         <v>22</v>
@@ -1186,7 +1186,7 @@
         <v>20</v>
       </c>
       <c r="B10">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C10" t="s">
         <v>21</v>
@@ -1992,7 +1992,7 @@
         <v>10</v>
       </c>
       <c r="B32">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C32" t="s">
         <v>136</v>
@@ -2030,7 +2030,7 @@
         <v>132</v>
       </c>
       <c r="B33">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C33" t="s">
         <v>62</v>
@@ -2220,7 +2220,7 @@
         <v>20</v>
       </c>
       <c r="B38">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C38" t="s">
         <v>210</v>
@@ -2296,7 +2296,7 @@
         <v>10</v>
       </c>
       <c r="B40">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C40" t="s">
         <v>61</v>
@@ -2334,7 +2334,7 @@
         <v>20</v>
       </c>
       <c r="B41">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C41">
         <v>0</v>

</xml_diff>

<commit_message>
Updates to BOM; added a board check firmware
</commit_message>
<xml_diff>
--- a/Inventory and Acquisitions/Master Inventory.xlsx
+++ b/Inventory and Acquisitions/Master Inventory.xlsx
@@ -147,9 +147,6 @@
     <t>20k</t>
   </si>
   <si>
-    <t>R301,R302,R303,R304,R305</t>
-  </si>
-  <si>
     <t>667-ERJ-3GEYJ203V</t>
   </si>
   <si>
@@ -650,6 +647,9 @@
   </si>
   <si>
     <t>2k (mistake)</t>
+  </si>
+  <si>
+    <t>R104,301,R302,R303,R304,R305</t>
   </si>
 </sst>
 </file>
@@ -1050,8 +1050,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1078,7 +1078,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B2" s="2"/>
     </row>
@@ -1102,7 +1102,7 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -1140,7 +1140,7 @@
         <v>9</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -1154,7 +1154,7 @@
         <v>22</v>
       </c>
       <c r="D9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E9" t="s">
         <v>12</v>
@@ -1172,13 +1172,13 @@
         <v>16</v>
       </c>
       <c r="J9" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K9" t="s">
         <v>18</v>
       </c>
       <c r="L9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -1210,13 +1210,13 @@
         <v>25</v>
       </c>
       <c r="J10" t="s">
+        <v>142</v>
+      </c>
+      <c r="K10" t="s">
+        <v>18</v>
+      </c>
+      <c r="L10" t="s">
         <v>143</v>
-      </c>
-      <c r="K10" t="s">
-        <v>18</v>
-      </c>
-      <c r="L10" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -1259,7 +1259,7 @@
         <v>36</v>
       </c>
       <c r="B12">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C12" t="s">
         <v>37</v>
@@ -1283,13 +1283,13 @@
         <v>41</v>
       </c>
       <c r="J12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="K12" t="s">
         <v>18</v>
       </c>
       <c r="L12" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -1297,13 +1297,13 @@
         <v>20</v>
       </c>
       <c r="B13">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C13" t="s">
         <v>42</v>
       </c>
       <c r="D13" t="s">
-        <v>43</v>
+        <v>210</v>
       </c>
       <c r="E13" t="s">
         <v>12</v>
@@ -1312,22 +1312,22 @@
         <v>13</v>
       </c>
       <c r="G13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H13" t="s">
         <v>24</v>
       </c>
       <c r="I13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J13" t="s">
+        <v>142</v>
+      </c>
+      <c r="K13" t="s">
+        <v>18</v>
+      </c>
+      <c r="L13" t="s">
         <v>143</v>
-      </c>
-      <c r="K13" t="s">
-        <v>18</v>
-      </c>
-      <c r="L13" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -1338,10 +1338,10 @@
         <v>10</v>
       </c>
       <c r="C14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E14" t="s">
         <v>12</v>
@@ -1350,22 +1350,22 @@
         <v>13</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H14" t="s">
         <v>24</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J14" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="K14" s="7" t="s">
         <v>18</v>
       </c>
       <c r="L14" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -1379,7 +1379,7 @@
         <v>22</v>
       </c>
       <c r="D15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E15" t="s">
         <v>12</v>
@@ -1388,22 +1388,22 @@
         <v>13</v>
       </c>
       <c r="G15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H15" t="s">
         <v>24</v>
       </c>
       <c r="I15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J15" t="s">
         <v>26</v>
       </c>
       <c r="K15" s="7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="L15" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -1414,10 +1414,10 @@
         <v>10</v>
       </c>
       <c r="C16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E16" t="s">
         <v>12</v>
@@ -1426,22 +1426,22 @@
         <v>13</v>
       </c>
       <c r="G16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H16" t="s">
         <v>24</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J16" s="7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="K16" s="7" t="s">
         <v>18</v>
       </c>
       <c r="L16" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -1452,10 +1452,10 @@
         <v>10</v>
       </c>
       <c r="C17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E17" t="s">
         <v>12</v>
@@ -1464,22 +1464,22 @@
         <v>13</v>
       </c>
       <c r="G17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H17" t="s">
         <v>24</v>
       </c>
       <c r="I17" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J17" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K17" s="7" t="s">
         <v>18</v>
       </c>
       <c r="L17" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -1487,13 +1487,13 @@
         <v>10</v>
       </c>
       <c r="B18">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D18" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E18" t="s">
         <v>12</v>
@@ -1502,22 +1502,22 @@
         <v>13</v>
       </c>
       <c r="G18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H18" t="s">
         <v>15</v>
       </c>
       <c r="I18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J18" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="K18" s="7" t="s">
         <v>18</v>
       </c>
       <c r="L18" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
@@ -1528,130 +1528,130 @@
         <v>12</v>
       </c>
       <c r="C19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D19" t="s">
+        <v>61</v>
+      </c>
+      <c r="E19" t="s">
         <v>62</v>
       </c>
-      <c r="E19" t="s">
-        <v>63</v>
-      </c>
       <c r="F19" s="9" t="s">
         <v>13</v>
       </c>
       <c r="G19" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H19" t="s">
         <v>15</v>
       </c>
       <c r="I19" t="s">
+        <v>104</v>
+      </c>
+      <c r="J19" t="s">
         <v>105</v>
       </c>
-      <c r="J19" t="s">
-        <v>106</v>
-      </c>
       <c r="K19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B20">
         <v>5</v>
       </c>
       <c r="C20" t="s">
+        <v>66</v>
+      </c>
+      <c r="D20" t="s">
         <v>67</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
+        <v>80</v>
+      </c>
+      <c r="F20" t="s">
+        <v>13</v>
+      </c>
+      <c r="G20" t="s">
         <v>68</v>
       </c>
-      <c r="E20" t="s">
-        <v>81</v>
-      </c>
-      <c r="F20" t="s">
-        <v>13</v>
-      </c>
-      <c r="G20" t="s">
+      <c r="H20" t="s">
         <v>69</v>
       </c>
-      <c r="H20" t="s">
+      <c r="I20" t="s">
         <v>70</v>
       </c>
-      <c r="I20" t="s">
-        <v>71</v>
-      </c>
       <c r="J20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K20" t="s">
         <v>18</v>
       </c>
       <c r="L20" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B21">
         <v>70</v>
       </c>
       <c r="C21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D21" t="s">
+        <v>72</v>
+      </c>
+      <c r="E21" t="s">
         <v>73</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
+        <v>13</v>
+      </c>
+      <c r="G21" t="s">
         <v>74</v>
       </c>
-      <c r="F21" t="s">
-        <v>13</v>
-      </c>
-      <c r="G21" t="s">
+      <c r="H21" t="s">
         <v>75</v>
       </c>
-      <c r="H21" t="s">
+      <c r="I21" t="s">
         <v>76</v>
       </c>
-      <c r="I21" t="s">
-        <v>77</v>
-      </c>
       <c r="J21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="K21" t="s">
         <v>18</v>
       </c>
       <c r="L21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B22">
         <v>7</v>
       </c>
       <c r="C22" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D22" t="s">
+        <v>78</v>
+      </c>
+      <c r="E22" t="s">
         <v>79</v>
       </c>
-      <c r="E22" t="s">
-        <v>80</v>
-      </c>
       <c r="H22" t="s">
+        <v>81</v>
+      </c>
+      <c r="I22" t="s">
         <v>82</v>
-      </c>
-      <c r="I22" t="s">
-        <v>83</v>
       </c>
       <c r="K22" t="s">
         <v>18</v>
@@ -1659,224 +1659,224 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B23">
         <v>4</v>
       </c>
       <c r="C23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D23" t="s">
+        <v>83</v>
+      </c>
+      <c r="E23" t="s">
         <v>84</v>
       </c>
-      <c r="E23" t="s">
+      <c r="F23" t="s">
+        <v>13</v>
+      </c>
+      <c r="G23" t="s">
         <v>85</v>
       </c>
-      <c r="F23" t="s">
-        <v>13</v>
-      </c>
-      <c r="G23" t="s">
+      <c r="H23" t="s">
+        <v>81</v>
+      </c>
+      <c r="I23" t="s">
         <v>86</v>
       </c>
-      <c r="H23" t="s">
-        <v>82</v>
-      </c>
-      <c r="I23" t="s">
-        <v>87</v>
-      </c>
       <c r="J23" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K23" t="s">
         <v>18</v>
       </c>
       <c r="L23" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B24">
         <v>4</v>
       </c>
       <c r="C24" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D24" t="s">
+        <v>89</v>
+      </c>
+      <c r="E24" t="s">
+        <v>93</v>
+      </c>
+      <c r="F24" t="s">
+        <v>13</v>
+      </c>
+      <c r="G24" t="s">
         <v>90</v>
       </c>
-      <c r="E24" t="s">
-        <v>94</v>
-      </c>
-      <c r="F24" t="s">
-        <v>13</v>
-      </c>
-      <c r="G24" t="s">
+      <c r="H24" t="s">
         <v>91</v>
       </c>
-      <c r="H24" t="s">
+      <c r="I24" t="s">
         <v>92</v>
       </c>
-      <c r="I24" t="s">
-        <v>93</v>
-      </c>
       <c r="J24" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K24" t="s">
         <v>18</v>
       </c>
       <c r="L24" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B25">
         <v>6</v>
       </c>
       <c r="C25" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D25" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E25" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F25" t="s">
         <v>13</v>
       </c>
       <c r="G25" t="s">
+        <v>95</v>
+      </c>
+      <c r="H25" t="s">
         <v>96</v>
       </c>
-      <c r="H25" t="s">
+      <c r="I25" t="s">
         <v>97</v>
       </c>
-      <c r="I25" t="s">
+      <c r="J25" t="s">
         <v>98</v>
       </c>
-      <c r="J25" t="s">
-        <v>99</v>
-      </c>
       <c r="K25" t="s">
         <v>18</v>
       </c>
       <c r="L25" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B26" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C26" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D26" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E26" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F26" t="s">
         <v>13</v>
       </c>
       <c r="G26" t="s">
+        <v>99</v>
+      </c>
+      <c r="H26" t="s">
         <v>100</v>
       </c>
-      <c r="H26" t="s">
+      <c r="I26" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="I26" s="5" t="s">
+      <c r="J26" t="s">
         <v>102</v>
       </c>
-      <c r="J26" t="s">
-        <v>103</v>
-      </c>
       <c r="K26" t="s">
         <v>18</v>
       </c>
       <c r="L26" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B27" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F27" t="s">
+        <v>109</v>
+      </c>
+      <c r="G27" t="s">
         <v>110</v>
       </c>
-      <c r="G27" t="s">
+      <c r="H27" t="s">
         <v>111</v>
       </c>
-      <c r="H27" t="s">
+      <c r="I27" t="s">
         <v>112</v>
       </c>
-      <c r="I27" t="s">
+      <c r="J27" t="s">
         <v>113</v>
       </c>
-      <c r="J27" t="s">
-        <v>114</v>
-      </c>
       <c r="K27" t="s">
         <v>18</v>
       </c>
       <c r="L27" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B28">
         <v>10</v>
       </c>
       <c r="C28" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D28" t="s">
+        <v>115</v>
+      </c>
+      <c r="E28" t="s">
+        <v>61</v>
+      </c>
+      <c r="F28" t="s">
         <v>116</v>
       </c>
-      <c r="E28" t="s">
-        <v>62</v>
-      </c>
-      <c r="F28" t="s">
-        <v>117</v>
-      </c>
       <c r="G28" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H28" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I28" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J28" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K28" t="s">
         <v>18</v>
@@ -1884,34 +1884,34 @@
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B29">
         <v>10</v>
       </c>
       <c r="C29" t="s">
+        <v>117</v>
+      </c>
+      <c r="D29" t="s">
         <v>118</v>
       </c>
-      <c r="D29" t="s">
-        <v>119</v>
-      </c>
       <c r="E29" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F29" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G29" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H29" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I29" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J29" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K29" t="s">
         <v>18</v>
@@ -1919,34 +1919,34 @@
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B30">
         <v>12</v>
       </c>
       <c r="C30" t="s">
+        <v>119</v>
+      </c>
+      <c r="D30" t="s">
         <v>120</v>
       </c>
-      <c r="D30" t="s">
-        <v>121</v>
-      </c>
       <c r="E30" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F30" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G30" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H30" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I30" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J30" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K30" t="s">
         <v>18</v>
@@ -1954,34 +1954,34 @@
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B31">
         <v>11</v>
       </c>
       <c r="C31" t="s">
+        <v>121</v>
+      </c>
+      <c r="D31" t="s">
         <v>122</v>
       </c>
-      <c r="D31" t="s">
-        <v>123</v>
-      </c>
       <c r="E31" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F31" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G31" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H31" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I31" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J31" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K31" t="s">
         <v>18</v>
@@ -1995,10 +1995,10 @@
         <v>10</v>
       </c>
       <c r="C32" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D32" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E32" t="s">
         <v>12</v>
@@ -2007,60 +2007,60 @@
         <v>13</v>
       </c>
       <c r="G32" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H32" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I32" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J32" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K32" t="s">
         <v>18</v>
       </c>
       <c r="L32" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B33">
         <v>4</v>
       </c>
       <c r="C33" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D33" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E33" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F33" t="s">
         <v>13</v>
       </c>
       <c r="G33" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H33" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I33" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J33" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="K33" t="s">
         <v>18</v>
       </c>
       <c r="L33" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
@@ -2071,10 +2071,10 @@
         <v>11</v>
       </c>
       <c r="C34" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D34" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E34" t="s">
         <v>12</v>
@@ -2083,22 +2083,22 @@
         <v>13</v>
       </c>
       <c r="G34" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H34" t="s">
         <v>15</v>
       </c>
       <c r="I34" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="J34" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K34" t="s">
         <v>18</v>
       </c>
       <c r="L34" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
@@ -2109,10 +2109,10 @@
         <v>10</v>
       </c>
       <c r="C35" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D35" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E35" t="s">
         <v>12</v>
@@ -2121,60 +2121,60 @@
         <v>13</v>
       </c>
       <c r="G35" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H35" t="s">
         <v>15</v>
       </c>
       <c r="I35" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="J35" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="K35" t="s">
         <v>18</v>
       </c>
       <c r="L35" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B36">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C36" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D36" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E36" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F36" t="s">
         <v>13</v>
       </c>
       <c r="G36" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H36" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I36" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J36" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="K36" t="s">
         <v>18</v>
       </c>
       <c r="L36" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
@@ -2185,7 +2185,7 @@
         <v>4</v>
       </c>
       <c r="C37" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D37" t="s">
         <v>38</v>
@@ -2197,22 +2197,22 @@
         <v>13</v>
       </c>
       <c r="G37" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H37" t="s">
         <v>15</v>
       </c>
       <c r="I37" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="J37" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="K37" t="s">
         <v>18</v>
       </c>
       <c r="L37" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
@@ -2223,10 +2223,10 @@
         <v>8</v>
       </c>
       <c r="C38" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D38" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E38" t="s">
         <v>12</v>
@@ -2235,22 +2235,22 @@
         <v>13</v>
       </c>
       <c r="G38" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H38" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I38" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J38" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="K38" t="s">
         <v>18</v>
       </c>
       <c r="L38" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
@@ -2258,13 +2258,13 @@
         <v>20</v>
       </c>
       <c r="B39">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C39">
         <v>180</v>
       </c>
       <c r="D39" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E39" t="s">
         <v>12</v>
@@ -2273,22 +2273,22 @@
         <v>13</v>
       </c>
       <c r="G39" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H39" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I39" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="J39" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="K39" t="s">
         <v>18</v>
       </c>
       <c r="L39" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
@@ -2299,10 +2299,10 @@
         <v>13</v>
       </c>
       <c r="C40" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D40" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E40" t="s">
         <v>12</v>
@@ -2311,22 +2311,22 @@
         <v>13</v>
       </c>
       <c r="G40" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="H40" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I40" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J40" s="9" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="K40" t="s">
         <v>18</v>
       </c>
       <c r="L40" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
@@ -2334,13 +2334,13 @@
         <v>20</v>
       </c>
       <c r="B41">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C41">
         <v>0</v>
       </c>
       <c r="D41" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E41" t="s">
         <v>12</v>
@@ -2349,112 +2349,112 @@
         <v>13</v>
       </c>
       <c r="G41" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H41" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I41" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J41" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="K41" t="s">
         <v>18</v>
       </c>
       <c r="L41" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B42">
         <v>3</v>
       </c>
       <c r="C42" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D42" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E42" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F42" t="s">
         <v>13</v>
       </c>
       <c r="G42" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H42" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I42" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="J42" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="K42" t="s">
         <v>18</v>
       </c>
       <c r="L42" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B43">
         <v>5</v>
       </c>
       <c r="C43" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D43" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E43" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F43" t="s">
         <v>13</v>
       </c>
       <c r="G43" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H43" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="I43" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="J43" s="9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="K43" t="s">
         <v>18</v>
       </c>
       <c r="L43" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B44">
         <v>9</v>
       </c>
       <c r="C44" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D44" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E44" t="s">
         <v>12</v>
@@ -2463,36 +2463,36 @@
         <v>13</v>
       </c>
       <c r="G44" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H44" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I44" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="J44" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K44" t="s">
         <v>18</v>
       </c>
       <c r="L44" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B45">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C45" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D45" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E45" t="s">
         <v>12</v>
@@ -2501,54 +2501,54 @@
         <v>13</v>
       </c>
       <c r="G45" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H45" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I45" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="J45" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K45" t="s">
         <v>18</v>
       </c>
       <c r="L45" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B46">
         <v>19</v>
       </c>
       <c r="C46" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D46" t="s">
+        <v>115</v>
+      </c>
+      <c r="E46" t="s">
+        <v>61</v>
+      </c>
+      <c r="F46" t="s">
         <v>116</v>
       </c>
-      <c r="E46" t="s">
-        <v>62</v>
-      </c>
-      <c r="F46" t="s">
-        <v>117</v>
-      </c>
       <c r="G46" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H46" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I46" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J46" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K46" t="s">
         <v>18</v>

</xml_diff>